<commit_message>
visualizzazione orari nel best planner e correzione bug nel calcolo del planner
</commit_message>
<xml_diff>
--- a/Template Upload.xlsx
+++ b/Template Upload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicholas.vittor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicholas.vittor\Desktop\Calendario\MB_Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672AE2C6-2AFB-427E-9C8E-F00C3E6A462F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96106E3E-5D96-46E4-9EA0-A84C593D3BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32655" yWindow="2760" windowWidth="23820" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -94,11 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -379,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,6 +391,7 @@
     <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="65.77734375" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" customWidth="1"/>
+    <col min="4" max="4" width="48.21875" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -407,6 +409,9 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>